<commit_message>
Replace logo with static ISS image. Replace 'Humans' with 'Total'. Changed fullscreen default for tkinter canvas. Add background color RGB variable
</commit_message>
<xml_diff>
--- a/humans_in_space/data/cumulative_space_visits_processed.xlsx
+++ b/humans_in_space/data/cumulative_space_visits_processed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattc\Documents\Python Scripts\Projects\data_viz\humans_in_space\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15DAAE6-3187-421D-BA86-8352E92E7124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B5B77B-F21B-4024-96CA-D29C87943903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12900" yWindow="4890" windowWidth="10470" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cum_visits" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>Misc</t>
   </si>
   <si>
-    <t>Humans</t>
-  </si>
-  <si>
     <t>Japanese</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>Russians</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,16 +901,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Replace logo with static ISS image. Replace 'Humans' with 'Total'. Changed fullscreen default for tkinter canvas. Add background color RGB variable (#2)
</commit_message>
<xml_diff>
--- a/humans_in_space/data/cumulative_space_visits_processed.xlsx
+++ b/humans_in_space/data/cumulative_space_visits_processed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattc\Documents\Python Scripts\Projects\data_viz\humans_in_space\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15DAAE6-3187-421D-BA86-8352E92E7124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B5B77B-F21B-4024-96CA-D29C87943903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12900" yWindow="4890" windowWidth="10470" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cum_visits" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>Misc</t>
   </si>
   <si>
-    <t>Humans</t>
-  </si>
-  <si>
     <t>Japanese</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>Russians</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,16 +901,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>

</xml_diff>